<commit_message>
Burndown Chart klar för andra sprinte samt ändringar
Lagt till Sprint Review & Retroperspective på både Sprint 1 och 2 samt
lagt till uppskattad tid på Product Backlog något jag gjorde i början
men vet ej varför den inte är kvar
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr dateCompatibility="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Blad1" state="visible" r:id="rId3"/>
+    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -38,40 +41,41 @@
   </si>
   <si>
     <t>Som användare vill jag kunna välja bild så att det visas på desktopen</t>
+  </si>
+  <si>
+    <t>Uppskattad Tid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -82,6 +86,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,57 +106,358 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="0" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" customWidth="1" max="1" width="1.43"/>
-    <col min="2" customWidth="1" max="2" width="70.14"/>
-    <col min="3" customWidth="1" max="3" width="12.43"/>
+    <col min="1" max="1" width="1.42578125" customWidth="1"/>
+    <col min="2" max="2" width="70.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c s="2" r="C1"/>
-      <c t="s" s="1" r="D1">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c t="s" r="B2">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="D2">
@@ -155,12 +466,15 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c t="s" r="B3">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
@@ -169,12 +483,15 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c t="s" r="B4">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
@@ -183,12 +500,15 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c t="s" r="B5">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
@@ -197,12 +517,15 @@
       <c r="E5">
         <v>2</v>
       </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c t="s" r="B6">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="D6">
@@ -211,7 +534,12 @@
       <c r="E6">
         <v>2</v>
       </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lagt till i Product Backlog
Lagt till Dokumentation samt Inlärning och hur lång tid de förväntades
ta
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Uppskattad Tid</t>
+  </si>
+  <si>
+    <t>Dokumentation</t>
+  </si>
+  <si>
+    <t>Inlärning</t>
   </si>
 </sst>
 </file>
@@ -422,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
   </cols>
@@ -538,6 +544,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>